<commit_message>
SMEMBERS, SDIFFSTORE, SINTERSTORE, SUNIONSTORE
</commit_message>
<xml_diff>
--- a/RedisCommands.xlsx
+++ b/RedisCommands.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="330">
   <si>
     <t>Group</t>
   </si>
@@ -972,6 +972,51 @@
   </si>
   <si>
     <t>HashScan</t>
+  </si>
+  <si>
+    <t>SetAddMemberStringAsync</t>
+  </si>
+  <si>
+    <t>SetAddMemberAsync</t>
+  </si>
+  <si>
+    <t>SetCardinalityAsync</t>
+  </si>
+  <si>
+    <t>SetGetDifferenceMembersStringAsync</t>
+  </si>
+  <si>
+    <t>SetGetDifferenceMembersAsync</t>
+  </si>
+  <si>
+    <t>SetStoreDifferenceMembersAsync</t>
+  </si>
+  <si>
+    <t>SetGetIntersectionMembersStringAsync</t>
+  </si>
+  <si>
+    <t>SetGetIntersectionMembersAsync</t>
+  </si>
+  <si>
+    <t>SetStoreIntersectionMembersAsync</t>
+  </si>
+  <si>
+    <t>SetGetUnionMembersStringAsync</t>
+  </si>
+  <si>
+    <t>SetGetUnionMembersAsync</t>
+  </si>
+  <si>
+    <t>SetStoreUnionMembersAsync</t>
+  </si>
+  <si>
+    <t>SetIsMemberAsync</t>
+  </si>
+  <si>
+    <t>SetGetMembersStringAsync</t>
+  </si>
+  <si>
+    <t>SetGetMembersAsync</t>
   </si>
 </sst>
 </file>
@@ -1326,8 +1371,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A201" sqref="A4:A201"/>
+    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
+      <selection activeCell="C173" sqref="C173:C174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3429,7 +3474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>256</v>
       </c>
@@ -3437,10 +3482,16 @@
         <v>257</v>
       </c>
       <c r="C161" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="D161" t="s">
+        <v>315</v>
+      </c>
+      <c r="E161" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>256</v>
       </c>
@@ -3448,10 +3499,13 @@
         <v>258</v>
       </c>
       <c r="C162" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="E162" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>256</v>
       </c>
@@ -3459,10 +3513,16 @@
         <v>259</v>
       </c>
       <c r="C163" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="D163" t="s">
+        <v>318</v>
+      </c>
+      <c r="E163" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>256</v>
       </c>
@@ -3470,10 +3530,13 @@
         <v>260</v>
       </c>
       <c r="C164" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="E164" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>256</v>
       </c>
@@ -3481,10 +3544,16 @@
         <v>261</v>
       </c>
       <c r="C165" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="D165" t="s">
+        <v>321</v>
+      </c>
+      <c r="E165" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>256</v>
       </c>
@@ -3492,10 +3561,13 @@
         <v>262</v>
       </c>
       <c r="C166" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="E166" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>256</v>
       </c>
@@ -3503,10 +3575,13 @@
         <v>263</v>
       </c>
       <c r="C167" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="E167" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>256</v>
       </c>
@@ -3514,10 +3589,16 @@
         <v>264</v>
       </c>
       <c r="C168" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="D168" t="s">
+        <v>328</v>
+      </c>
+      <c r="E168" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>256</v>
       </c>
@@ -3528,7 +3609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>256</v>
       </c>
@@ -3539,7 +3620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>256</v>
       </c>
@@ -3550,7 +3631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>256</v>
       </c>
@@ -3561,7 +3642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>256</v>
       </c>
@@ -3569,10 +3650,16 @@
         <v>269</v>
       </c>
       <c r="C173" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="D173" t="s">
+        <v>324</v>
+      </c>
+      <c r="E173" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>256</v>
       </c>
@@ -3580,10 +3667,13 @@
         <v>270</v>
       </c>
       <c r="C174" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="E174" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>256</v>
       </c>
@@ -3594,7 +3684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>272</v>
       </c>

</xml_diff>

<commit_message>
Update redis commands list.
</commit_message>
<xml_diff>
--- a/RedisCommands.xlsx
+++ b/RedisCommands.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="10185"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25610" windowHeight="10190"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="344">
   <si>
     <t>Group</t>
   </si>
@@ -1044,6 +1044,21 @@
   </si>
   <si>
     <t>SetScanAsync</t>
+  </si>
+  <si>
+    <t>SortedSetAddMembersAsync, SortedSetAddOnlyMembersAsync, SortedSetUpsertMembersAsync, SortedSetUpdateMembersAsync</t>
+  </si>
+  <si>
+    <t>SortedSetAddMembersStringAsync, SortedSetAddOnlyMembersStringAsync, SortedSetUpsertMembersStringAsync, SortedSetUpdateMembersStringAsync</t>
+  </si>
+  <si>
+    <t>SortedSetCardinalityAsync</t>
+  </si>
+  <si>
+    <t>SortedSetGetScoreAsync</t>
+  </si>
+  <si>
+    <t>SortedSetGetScoreStringAsync</t>
   </si>
 </sst>
 </file>
@@ -1398,18 +1413,16 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E175" sqref="E175"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="24.140625" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.1796875" customWidth="1"/>
+    <col min="4" max="4" width="121.1796875" customWidth="1"/>
     <col min="6" max="6" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1429,7 +1442,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1443,7 +1456,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1457,7 +1470,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1468,7 +1481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1482,7 +1495,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1496,7 +1509,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1510,7 +1523,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1524,7 +1537,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1541,7 +1554,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1555,7 +1568,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1572,7 +1585,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1589,7 +1602,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1603,7 +1616,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -1617,7 +1630,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1631,7 +1644,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -1648,7 +1661,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -1665,7 +1678,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -1682,7 +1695,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -1696,7 +1709,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -1713,7 +1726,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -1727,7 +1740,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -1741,7 +1754,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -1755,7 +1768,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -1772,7 +1785,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -1786,7 +1799,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -1800,7 +1813,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>55</v>
       </c>
@@ -1811,7 +1824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>55</v>
       </c>
@@ -1825,7 +1838,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>55</v>
       </c>
@@ -1839,7 +1852,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>55</v>
       </c>
@@ -1853,7 +1866,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>55</v>
       </c>
@@ -1867,7 +1880,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>55</v>
       </c>
@@ -1878,7 +1891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>55</v>
       </c>
@@ -1892,7 +1905,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>55</v>
       </c>
@@ -1903,7 +1916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>55</v>
       </c>
@@ -1917,7 +1930,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>55</v>
       </c>
@@ -1931,7 +1944,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>55</v>
       </c>
@@ -1945,7 +1958,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>55</v>
       </c>
@@ -1959,7 +1972,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>55</v>
       </c>
@@ -1973,7 +1986,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>55</v>
       </c>
@@ -1987,7 +2000,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>55</v>
       </c>
@@ -2001,7 +2014,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>55</v>
       </c>
@@ -2012,7 +2025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>55</v>
       </c>
@@ -2023,7 +2036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>55</v>
       </c>
@@ -2037,7 +2050,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>55</v>
       </c>
@@ -2051,7 +2064,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>55</v>
       </c>
@@ -2065,7 +2078,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>55</v>
       </c>
@@ -2076,7 +2089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>55</v>
       </c>
@@ -2087,7 +2100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>55</v>
       </c>
@@ -2101,7 +2114,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>94</v>
       </c>
@@ -2115,7 +2128,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>94</v>
       </c>
@@ -2129,7 +2142,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>94</v>
       </c>
@@ -2146,7 +2159,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>94</v>
       </c>
@@ -2163,7 +2176,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>94</v>
       </c>
@@ -2177,7 +2190,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>94</v>
       </c>
@@ -2191,7 +2204,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>94</v>
       </c>
@@ -2205,7 +2218,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>94</v>
       </c>
@@ -2219,7 +2232,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>94</v>
       </c>
@@ -2236,7 +2249,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>94</v>
       </c>
@@ -2253,7 +2266,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>94</v>
       </c>
@@ -2270,7 +2283,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>94</v>
       </c>
@@ -2287,7 +2300,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>94</v>
       </c>
@@ -2301,7 +2314,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>94</v>
       </c>
@@ -2318,7 +2331,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>94</v>
       </c>
@@ -2335,7 +2348,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>128</v>
       </c>
@@ -2352,7 +2365,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>128</v>
       </c>
@@ -2369,7 +2382,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>128</v>
       </c>
@@ -2386,7 +2399,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>128</v>
       </c>
@@ -2403,7 +2416,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>128</v>
       </c>
@@ -2420,7 +2433,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>128</v>
       </c>
@@ -2434,7 +2447,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>128</v>
       </c>
@@ -2451,7 +2464,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>128</v>
       </c>
@@ -2468,7 +2481,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>128</v>
       </c>
@@ -2485,7 +2498,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>128</v>
       </c>
@@ -2502,7 +2515,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>128</v>
       </c>
@@ -2519,7 +2532,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>128</v>
       </c>
@@ -2536,7 +2549,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>128</v>
       </c>
@@ -2550,7 +2563,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>128</v>
       </c>
@@ -2567,7 +2580,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>128</v>
       </c>
@@ -2584,7 +2597,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>128</v>
       </c>
@@ -2601,7 +2614,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>128</v>
       </c>
@@ -2618,7 +2631,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>164</v>
       </c>
@@ -2629,7 +2642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>164</v>
       </c>
@@ -2640,7 +2653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>164</v>
       </c>
@@ -2651,7 +2664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>164</v>
       </c>
@@ -2662,7 +2675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>164</v>
       </c>
@@ -2673,7 +2686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>164</v>
       </c>
@@ -2684,7 +2697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>164</v>
       </c>
@@ -2695,7 +2708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>164</v>
       </c>
@@ -2706,7 +2719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>164</v>
       </c>
@@ -2717,7 +2730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>164</v>
       </c>
@@ -2728,7 +2741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>164</v>
       </c>
@@ -2739,7 +2752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>164</v>
       </c>
@@ -2750,7 +2763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>164</v>
       </c>
@@ -2761,7 +2774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>164</v>
       </c>
@@ -2772,7 +2785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>164</v>
       </c>
@@ -2783,7 +2796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>164</v>
       </c>
@@ -2794,7 +2807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>164</v>
       </c>
@@ -2805,7 +2818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>164</v>
       </c>
@@ -2816,7 +2829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>164</v>
       </c>
@@ -2827,7 +2840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>164</v>
       </c>
@@ -2838,7 +2851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>164</v>
       </c>
@@ -2849,7 +2862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>164</v>
       </c>
@@ -2860,7 +2873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>164</v>
       </c>
@@ -2871,7 +2884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>164</v>
       </c>
@@ -2882,7 +2895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>164</v>
       </c>
@@ -2893,7 +2906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>164</v>
       </c>
@@ -2904,7 +2917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>164</v>
       </c>
@@ -2915,7 +2928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>164</v>
       </c>
@@ -2926,7 +2939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>164</v>
       </c>
@@ -2937,7 +2950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>164</v>
       </c>
@@ -2948,7 +2961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>164</v>
       </c>
@@ -2959,7 +2972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>196</v>
       </c>
@@ -2973,7 +2986,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>196</v>
       </c>
@@ -2987,7 +3000,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>196</v>
       </c>
@@ -3001,7 +3014,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>196</v>
       </c>
@@ -3015,7 +3028,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>196</v>
       </c>
@@ -3029,7 +3042,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>196</v>
       </c>
@@ -3040,7 +3053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>208</v>
       </c>
@@ -3051,7 +3064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>208</v>
       </c>
@@ -3062,7 +3075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>208</v>
       </c>
@@ -3073,7 +3086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>208</v>
       </c>
@@ -3084,7 +3097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>208</v>
       </c>
@@ -3095,7 +3108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>208</v>
       </c>
@@ -3106,7 +3119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>208</v>
       </c>
@@ -3117,7 +3130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>208</v>
       </c>
@@ -3128,7 +3141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>208</v>
       </c>
@@ -3139,7 +3152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>208</v>
       </c>
@@ -3150,7 +3163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>208</v>
       </c>
@@ -3161,7 +3174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>208</v>
       </c>
@@ -3172,7 +3185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>208</v>
       </c>
@@ -3183,7 +3196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>208</v>
       </c>
@@ -3194,7 +3207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>208</v>
       </c>
@@ -3205,7 +3218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>208</v>
       </c>
@@ -3216,7 +3229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>208</v>
       </c>
@@ -3227,7 +3240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>208</v>
       </c>
@@ -3238,7 +3251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>208</v>
       </c>
@@ -3249,7 +3262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>208</v>
       </c>
@@ -3260,7 +3273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>229</v>
       </c>
@@ -3271,7 +3284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>229</v>
       </c>
@@ -3282,7 +3295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>229</v>
       </c>
@@ -3293,7 +3306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>229</v>
       </c>
@@ -3304,7 +3317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>229</v>
       </c>
@@ -3315,7 +3328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>229</v>
       </c>
@@ -3326,7 +3339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>236</v>
       </c>
@@ -3337,7 +3350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>236</v>
       </c>
@@ -3348,7 +3361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>236</v>
       </c>
@@ -3359,7 +3372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>241</v>
       </c>
@@ -3370,7 +3383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>241</v>
       </c>
@@ -3381,7 +3394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>241</v>
       </c>
@@ -3392,7 +3405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>241</v>
       </c>
@@ -3403,7 +3416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>241</v>
       </c>
@@ -3414,7 +3427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>241</v>
       </c>
@@ -3425,7 +3438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>248</v>
       </c>
@@ -3436,7 +3449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>248</v>
       </c>
@@ -3447,7 +3460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>248</v>
       </c>
@@ -3458,7 +3471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>248</v>
       </c>
@@ -3469,7 +3482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>248</v>
       </c>
@@ -3480,7 +3493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>248</v>
       </c>
@@ -3491,7 +3504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>248</v>
       </c>
@@ -3502,7 +3515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>256</v>
       </c>
@@ -3519,7 +3532,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="162" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>256</v>
       </c>
@@ -3533,7 +3546,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="163" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>256</v>
       </c>
@@ -3550,7 +3563,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="164" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>256</v>
       </c>
@@ -3564,7 +3577,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="165" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>256</v>
       </c>
@@ -3581,7 +3594,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="166" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>256</v>
       </c>
@@ -3595,7 +3608,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="167" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>256</v>
       </c>
@@ -3609,7 +3622,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="168" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>256</v>
       </c>
@@ -3626,7 +3639,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>256</v>
       </c>
@@ -3643,7 +3656,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>256</v>
       </c>
@@ -3660,7 +3673,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>256</v>
       </c>
@@ -3677,7 +3690,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>256</v>
       </c>
@@ -3694,7 +3707,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="173" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>256</v>
       </c>
@@ -3711,7 +3724,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="174" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>256</v>
       </c>
@@ -3725,7 +3738,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>256</v>
       </c>
@@ -3739,7 +3752,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="176" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>272</v>
       </c>
@@ -3747,10 +3760,16 @@
         <v>273</v>
       </c>
       <c r="C176" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D176" t="s">
+        <v>340</v>
+      </c>
+      <c r="E176" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>272</v>
       </c>
@@ -3758,10 +3777,13 @@
         <v>274</v>
       </c>
       <c r="C177" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E177" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>272</v>
       </c>
@@ -3772,7 +3794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>272</v>
       </c>
@@ -3783,7 +3805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>272</v>
       </c>
@@ -3794,7 +3816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>272</v>
       </c>
@@ -3805,7 +3827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>272</v>
       </c>
@@ -3816,7 +3838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>272</v>
       </c>
@@ -3827,7 +3849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>272</v>
       </c>
@@ -3838,7 +3860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>272</v>
       </c>
@@ -3849,7 +3871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>272</v>
       </c>
@@ -3860,7 +3882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>272</v>
       </c>
@@ -3871,7 +3893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>272</v>
       </c>
@@ -3882,7 +3904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>272</v>
       </c>
@@ -3893,7 +3915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>272</v>
       </c>
@@ -3904,7 +3926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>272</v>
       </c>
@@ -3915,7 +3937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>272</v>
       </c>
@@ -3926,7 +3948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>272</v>
       </c>
@@ -3937,7 +3959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>272</v>
       </c>
@@ -3945,10 +3967,16 @@
         <v>290</v>
       </c>
       <c r="C194" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D194" t="s">
+        <v>343</v>
+      </c>
+      <c r="E194" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>272</v>
       </c>
@@ -3959,7 +3987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>272</v>
       </c>
@@ -3970,7 +3998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>294</v>
       </c>
@@ -3981,7 +4009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>294</v>
       </c>
@@ -3992,7 +4020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>294</v>
       </c>
@@ -4003,7 +4031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>294</v>
       </c>
@@ -4014,7 +4042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>294</v>
       </c>
@@ -4029,12 +4057,7 @@
   <autoFilter ref="A1:F201">
     <filterColumn colId="0">
       <filters>
-        <filter val="Sets"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="FALSE"/>
+        <filter val="Sorted Sets"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
ZCOUNT, ZINCRBY, ZINTERSTORE, ZUNIONSTORE
</commit_message>
<xml_diff>
--- a/RedisCommands.xlsx
+++ b/RedisCommands.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="349">
   <si>
     <t>Group</t>
   </si>
@@ -1059,6 +1059,21 @@
   </si>
   <si>
     <t>SortedSetGetScoreStringAsync</t>
+  </si>
+  <si>
+    <t>SortedSetGetCountAsync</t>
+  </si>
+  <si>
+    <t>SortedSetIncrementByStringAsync</t>
+  </si>
+  <si>
+    <t>SortedSetIncrementByAsync</t>
+  </si>
+  <si>
+    <t>SortedSetStoreIntersectionMembersAsync</t>
+  </si>
+  <si>
+    <t>SortedSetStoreUnionMembersAsync</t>
   </si>
 </sst>
 </file>
@@ -1413,7 +1428,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D192" sqref="D192"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -3791,7 +3808,10 @@
         <v>275</v>
       </c>
       <c r="C178" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E178" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.35">
@@ -3802,7 +3822,13 @@
         <v>276</v>
       </c>
       <c r="C179" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D179" t="s">
+        <v>345</v>
+      </c>
+      <c r="E179" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.35">
@@ -3813,7 +3839,10 @@
         <v>277</v>
       </c>
       <c r="C180" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E180" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.35">
@@ -3984,7 +4013,10 @@
         <v>291</v>
       </c>
       <c r="C195" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E195" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
ZLEXCOUNT, ZRANGE, ZRANGEBYLEX, ZRANGEBYSCORE, ZREVRANGE, ZREVRANGEBYLEX, ZREVRANGEBYSCORE
</commit_message>
<xml_diff>
--- a/RedisCommands.xlsx
+++ b/RedisCommands.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="360">
   <si>
     <t>Group</t>
   </si>
@@ -1074,6 +1074,39 @@
   </si>
   <si>
     <t>SortedSetStoreUnionMembersAsync</t>
+  </si>
+  <si>
+    <t>SortedSetGetLexCountAsync</t>
+  </si>
+  <si>
+    <t>SortedSetGetRangeStringAsync, SortedSetGetRangeWithScoresStringAsync</t>
+  </si>
+  <si>
+    <t>SortedSetGetRangeAsync, SortedSetGetRangeWithScoresAsync</t>
+  </si>
+  <si>
+    <t>SortedSetGetLexRangeAsync</t>
+  </si>
+  <si>
+    <t>SortedSetGetReverseLexRangeAsync</t>
+  </si>
+  <si>
+    <t>SortedSetGetRangeByScoreStringAsync, SortedSetGetRangeByScoreWithScoresStringAsync</t>
+  </si>
+  <si>
+    <t>SortedSetGetRangeByScoreAsync, SortedSetGetRangeByScoreWithScoresAsync</t>
+  </si>
+  <si>
+    <t>SortedSetGetReverseRangeStringAsync, SortedSetGetReverseRangeWithScoresStringAsync</t>
+  </si>
+  <si>
+    <t>SortedSetGetReverseRangeAsync, SortedSetGetReverseRangeWithScoresAsync</t>
+  </si>
+  <si>
+    <t>SortedSetGetReverseRangeByScoreStringAsync, SortedSetGetReverseRangeByScoreWithScoresStringAsync</t>
+  </si>
+  <si>
+    <t>SortedSetGetReverseRangeByScoreAsync, SortedSetGetReverseRangeByScoreWithScoresAsync</t>
   </si>
 </sst>
 </file>
@@ -1429,7 +1462,7 @@
   <dimension ref="A1:F201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D192" sqref="D192"/>
+      <selection activeCell="B192" activeCellId="2" sqref="B181:B185 B191 B192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3853,7 +3886,10 @@
         <v>278</v>
       </c>
       <c r="C181" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D181" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.35">
@@ -3864,7 +3900,13 @@
         <v>279</v>
       </c>
       <c r="C182" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D182" t="s">
+        <v>350</v>
+      </c>
+      <c r="E182" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.35">
@@ -3875,7 +3917,10 @@
         <v>280</v>
       </c>
       <c r="C183" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D183" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.35">
@@ -3886,7 +3931,10 @@
         <v>281</v>
       </c>
       <c r="C184" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D184" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.35">
@@ -3897,7 +3945,13 @@
         <v>282</v>
       </c>
       <c r="C185" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D185" t="s">
+        <v>354</v>
+      </c>
+      <c r="E185" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.35">
@@ -3963,7 +4017,13 @@
         <v>293</v>
       </c>
       <c r="C191" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D191" t="s">
+        <v>356</v>
+      </c>
+      <c r="E191" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.35">
@@ -3974,7 +4034,13 @@
         <v>288</v>
       </c>
       <c r="C192" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D192" t="s">
+        <v>358</v>
+      </c>
+      <c r="E192" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
ZREM, ZREMRANGEBYLEX, ZREMRANGEBYRANK, ZREMRANGEBYSCORE
</commit_message>
<xml_diff>
--- a/RedisCommands.xlsx
+++ b/RedisCommands.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="369">
   <si>
     <t>Group</t>
   </si>
@@ -1119,6 +1119,21 @@
   </si>
   <si>
     <t>SortedSetGetRankStringAsync</t>
+  </si>
+  <si>
+    <t>SortedSetRemoveRangeByLexAsync</t>
+  </si>
+  <si>
+    <t>SortedSetRemoveRangeByRankAsync</t>
+  </si>
+  <si>
+    <t>SortedSetRemoveRangeByScoreAsync</t>
+  </si>
+  <si>
+    <t>SortedSetRemoveMembersAsync</t>
+  </si>
+  <si>
+    <t>SortedSetRemoveMembersStringAsync</t>
   </si>
 </sst>
 </file>
@@ -1474,7 +1489,7 @@
   <dimension ref="A1:F201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D195" sqref="D195"/>
+      <selection activeCell="B187" sqref="B187:B190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3991,7 +4006,13 @@
         <v>284</v>
       </c>
       <c r="C187" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D187" t="s">
+        <v>368</v>
+      </c>
+      <c r="E187" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.35">
@@ -4002,7 +4023,10 @@
         <v>285</v>
       </c>
       <c r="C188" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D188" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.35">
@@ -4013,7 +4037,10 @@
         <v>286</v>
       </c>
       <c r="C189" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E189" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.35">
@@ -4024,7 +4051,10 @@
         <v>287</v>
       </c>
       <c r="C190" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E190" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
INFO, BGSAVE, SAVE, CONFIG GET/SET/RESETSTATS/REWRITE, BGREWRITEAOF, LASTSAVE, DBSIZE, FLUSHDB, FLUSHALL
</commit_message>
<xml_diff>
--- a/RedisCommands.xlsx
+++ b/RedisCommands.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="393">
   <si>
     <t>Group</t>
   </si>
@@ -1164,6 +1164,48 @@
   </si>
   <si>
     <t>Not to be implemented by clients.</t>
+  </si>
+  <si>
+    <t>FlushAllAsync</t>
+  </si>
+  <si>
+    <t>FlushDatabaseAsync</t>
+  </si>
+  <si>
+    <t>No plans, requires streaming</t>
+  </si>
+  <si>
+    <t>GetDatabaseSizeAsync</t>
+  </si>
+  <si>
+    <t>No plans</t>
+  </si>
+  <si>
+    <t>SetConfigurationAsync</t>
+  </si>
+  <si>
+    <t>GetConfigurationAsync</t>
+  </si>
+  <si>
+    <t>ResetConfigurationStatsAsync</t>
+  </si>
+  <si>
+    <t>RewriteConfigurationAsync</t>
+  </si>
+  <si>
+    <t>BackgroundSaveAsync</t>
+  </si>
+  <si>
+    <t>SaveAsync</t>
+  </si>
+  <si>
+    <t>BackgroundRewriteAppendOnlyFileAsync</t>
+  </si>
+  <si>
+    <t>GetLastSaveDateTimeAsync</t>
+  </si>
+  <si>
+    <t>GetServerInformationAsync</t>
   </si>
 </sst>
 </file>
@@ -1518,8 +1560,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D109" sqref="D109"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="C120" sqref="C120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2758,7 +2800,10 @@
         <v>165</v>
       </c>
       <c r="C82" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E82" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
@@ -2769,7 +2814,10 @@
         <v>166</v>
       </c>
       <c r="C83" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E83" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
@@ -2899,7 +2947,10 @@
         <v>177</v>
       </c>
       <c r="C94" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E94" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.35">
@@ -2910,7 +2961,10 @@
         <v>178</v>
       </c>
       <c r="C95" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E95" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.35">
@@ -2921,7 +2975,10 @@
         <v>179</v>
       </c>
       <c r="C96" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E96" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.35">
@@ -2932,7 +2989,10 @@
         <v>180</v>
       </c>
       <c r="C97" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E97" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2943,7 +3003,10 @@
         <v>181</v>
       </c>
       <c r="C98" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E98" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.35">
@@ -2982,7 +3045,10 @@
         <v>184</v>
       </c>
       <c r="C101" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E101" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.35">
@@ -2993,7 +3059,10 @@
         <v>185</v>
       </c>
       <c r="C102" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E102" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.35">
@@ -3004,7 +3073,10 @@
         <v>186</v>
       </c>
       <c r="C103" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E103" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.35">
@@ -3015,7 +3087,10 @@
         <v>187</v>
       </c>
       <c r="C104" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E104" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.35">
@@ -3028,6 +3103,9 @@
       <c r="C105" t="b">
         <v>0</v>
       </c>
+      <c r="F105" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
@@ -3048,7 +3126,10 @@
         <v>190</v>
       </c>
       <c r="C107" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E107" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.35">
@@ -3060,6 +3141,9 @@
       </c>
       <c r="C108" t="b">
         <v>0</v>
+      </c>
+      <c r="F108" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
GEOADD, GEOPOS, GEOHASH, GEODISTANCE
</commit_message>
<xml_diff>
--- a/RedisCommands.xlsx
+++ b/RedisCommands.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="398">
   <si>
     <t>Group</t>
   </si>
@@ -1206,6 +1206,21 @@
   </si>
   <si>
     <t>GetServerInformationAsync</t>
+  </si>
+  <si>
+    <t>SKIP</t>
+  </si>
+  <si>
+    <t>GeoAddAsync</t>
+  </si>
+  <si>
+    <t>GeoPositionAsync</t>
+  </si>
+  <si>
+    <t>GeoHashAsync</t>
+  </si>
+  <si>
+    <t>GeoDistanceAsync</t>
   </si>
 </sst>
 </file>
@@ -1560,8 +1575,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="C120" sqref="C120"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C142" sqref="C142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1844,15 +1859,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>3</v>
       </c>
       <c r="B19" t="s">
         <v>25</v>
       </c>
-      <c r="C19" t="b">
-        <v>0</v>
+      <c r="C19" t="s">
+        <v>393</v>
       </c>
       <c r="F19" t="s">
         <v>51</v>
@@ -1889,29 +1904,29 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>3</v>
       </c>
       <c r="B22" t="s">
         <v>28</v>
       </c>
-      <c r="C22" t="b">
-        <v>0</v>
+      <c r="C22" t="s">
+        <v>393</v>
       </c>
       <c r="F22" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>3</v>
       </c>
       <c r="B23" t="s">
         <v>29</v>
       </c>
-      <c r="C23" t="b">
-        <v>0</v>
+      <c r="C23" t="s">
+        <v>393</v>
       </c>
       <c r="F23" t="s">
         <v>51</v>
@@ -1962,7 +1977,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>55</v>
       </c>
@@ -2065,7 +2080,7 @@
         <v>64</v>
       </c>
       <c r="C34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E34" t="s">
         <v>372</v>
@@ -2169,7 +2184,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>55</v>
       </c>
@@ -2183,7 +2198,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>55</v>
       </c>
@@ -2792,7 +2807,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>164</v>
       </c>
@@ -2806,7 +2821,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>164</v>
       </c>
@@ -2831,7 +2846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>164</v>
       </c>
@@ -2845,7 +2860,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>164</v>
       </c>
@@ -2881,7 +2896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>164</v>
       </c>
@@ -2939,7 +2954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>164</v>
       </c>
@@ -2953,7 +2968,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>164</v>
       </c>
@@ -2967,7 +2982,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>164</v>
       </c>
@@ -2981,7 +2996,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>164</v>
       </c>
@@ -2995,7 +3010,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:6" ht="29.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>164</v>
       </c>
@@ -3009,35 +3024,35 @@
         <v>382</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>164</v>
       </c>
       <c r="B99" t="s">
         <v>182</v>
       </c>
-      <c r="C99" t="b">
-        <v>0</v>
+      <c r="C99" t="s">
+        <v>393</v>
       </c>
       <c r="F99" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>164</v>
       </c>
       <c r="B100" t="s">
         <v>183</v>
       </c>
-      <c r="C100" t="b">
-        <v>0</v>
+      <c r="C100" t="s">
+        <v>393</v>
       </c>
       <c r="F100" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>164</v>
       </c>
@@ -3051,7 +3066,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>164</v>
       </c>
@@ -3065,7 +3080,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>164</v>
       </c>
@@ -3079,7 +3094,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>164</v>
       </c>
@@ -3093,15 +3108,15 @@
         <v>391</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>164</v>
       </c>
       <c r="B105" t="s">
         <v>188</v>
       </c>
-      <c r="C105" t="b">
-        <v>0</v>
+      <c r="C105" t="s">
+        <v>393</v>
       </c>
       <c r="F105" t="s">
         <v>381</v>
@@ -3118,7 +3133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>164</v>
       </c>
@@ -3132,15 +3147,15 @@
         <v>389</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>164</v>
       </c>
       <c r="B108" t="s">
         <v>191</v>
       </c>
-      <c r="C108" t="b">
-        <v>0</v>
+      <c r="C108" t="s">
+        <v>393</v>
       </c>
       <c r="F108" t="s">
         <v>383</v>
@@ -3179,7 +3194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>164</v>
       </c>
@@ -3384,7 +3399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>208</v>
       </c>
@@ -3395,7 +3410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>208</v>
       </c>
@@ -3406,7 +3421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>208</v>
       </c>
@@ -3417,7 +3432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>208</v>
       </c>
@@ -3428,7 +3443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>208</v>
       </c>
@@ -3439,7 +3454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>208</v>
       </c>
@@ -3450,7 +3465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>208</v>
       </c>
@@ -3461,7 +3476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>208</v>
       </c>
@@ -3472,7 +3487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>208</v>
       </c>
@@ -3483,7 +3498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>208</v>
       </c>
@@ -3494,7 +3509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>229</v>
       </c>
@@ -3502,10 +3517,13 @@
         <v>230</v>
       </c>
       <c r="C139" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="E139" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>229</v>
       </c>
@@ -3513,10 +3531,13 @@
         <v>231</v>
       </c>
       <c r="C140" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="E140" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>229</v>
       </c>
@@ -3524,10 +3545,13 @@
         <v>232</v>
       </c>
       <c r="C141" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="E141" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>229</v>
       </c>
@@ -3535,10 +3559,13 @@
         <v>233</v>
       </c>
       <c r="C142" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="E142" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>229</v>
       </c>
@@ -3549,7 +3576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>229</v>
       </c>

</xml_diff>

<commit_message>
GEORADIUSBYMEMBER, PFADD, PFCOUNT, PFMERGE
</commit_message>
<xml_diff>
--- a/RedisCommands.xlsx
+++ b/RedisCommands.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="403">
   <si>
     <t>Group</t>
   </si>
@@ -1224,6 +1224,18 @@
   </si>
   <si>
     <t>GeoRadius</t>
+  </si>
+  <si>
+    <t>HyperLogLogAddAsync</t>
+  </si>
+  <si>
+    <t>HyperLogLogCountAsync</t>
+  </si>
+  <si>
+    <t>HyperLogLogAddStringAsync</t>
+  </si>
+  <si>
+    <t>HyperLogLogMergeAsync</t>
   </si>
 </sst>
 </file>
@@ -1578,8 +1590,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="C143" sqref="C143"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="C160" sqref="C160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2075,7 +2087,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>55</v>
       </c>
@@ -3512,7 +3524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>229</v>
       </c>
@@ -3526,7 +3538,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>229</v>
       </c>
@@ -3540,7 +3552,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>229</v>
       </c>
@@ -3554,7 +3566,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>229</v>
       </c>
@@ -3568,7 +3580,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>229</v>
       </c>
@@ -3582,7 +3594,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>229</v>
       </c>
@@ -3590,10 +3602,13 @@
         <v>235</v>
       </c>
       <c r="C144" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="E144" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>236</v>
       </c>
@@ -3601,10 +3616,16 @@
         <v>237</v>
       </c>
       <c r="C145" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="D145" t="s">
+        <v>401</v>
+      </c>
+      <c r="E145" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>236</v>
       </c>
@@ -3612,10 +3633,13 @@
         <v>238</v>
       </c>
       <c r="C146" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="E146" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>236</v>
       </c>
@@ -3623,10 +3647,13 @@
         <v>239</v>
       </c>
       <c r="C147" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="E147" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>241</v>
       </c>
@@ -3637,7 +3664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>241</v>
       </c>
@@ -3648,7 +3675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>241</v>
       </c>
@@ -3659,7 +3686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>241</v>
       </c>
@@ -3670,7 +3697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>241</v>
       </c>
@@ -3681,7 +3708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>241</v>
       </c>
@@ -3692,7 +3719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>248</v>
       </c>
@@ -3703,7 +3730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>248</v>
       </c>
@@ -3714,7 +3741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>248</v>
       </c>
@@ -3725,7 +3752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>248</v>
       </c>
@@ -3736,7 +3763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>248</v>
       </c>
@@ -3747,7 +3774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>248</v>
       </c>
@@ -3758,7 +3785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>248</v>
       </c>

</xml_diff>